<commit_message>
Data Understanding 1 and 2
</commit_message>
<xml_diff>
--- a/Variables Overview.xlsx
+++ b/Variables Overview.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\Documents\Michele_FHNW\Semester_8\Time Series Analysis with R\R_Files\Data-Analytics-Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F22F49-A3E4-4566-B318-70A70783EE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,158 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+  <si>
+    <t>Variable name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Unique Values</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>chr</t>
+  </si>
+  <si>
+    <t>Marital</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Average yearly balance</t>
+  </si>
+  <si>
+    <t>NOT in the data</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Loan</t>
+  </si>
+  <si>
+    <t>Day_of_week</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Campaign</t>
+  </si>
+  <si>
+    <t>Number of contacts performed during this campaign and for this client</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>Number of contacts performed before this campaign and for this client</t>
+  </si>
+  <si>
+    <t>Poutcome</t>
+  </si>
+  <si>
+    <t>Emp.var.rate</t>
+  </si>
+  <si>
+    <t>Employment variation rate – quarterly indicator</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>Cons.price.idx</t>
+  </si>
+  <si>
+    <t>Consumer price index – monthly indicator</t>
+  </si>
+  <si>
+    <t>Cons.conf.idx</t>
+  </si>
+  <si>
+    <t>Consumer confidence index – monthly indicator</t>
+  </si>
+  <si>
+    <t>Euribor3m</t>
+  </si>
+  <si>
+    <t>Euribor 3-month rate – daily indicator</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Type of job (categorical: 'admin.', 'blue-collar', 'entrepreneur', 'housemaid', 'management', 'retired', 'self-employed', 'services', 'student', 'technician', 'unemployed', 'unknown')</t>
+  </si>
+  <si>
+    <t>Marital status (categorical: 'divorced', 'married', 'single', 'unknown')note: 'divorced' means divorced or widowed</t>
+  </si>
+  <si>
+    <t>Education level (categorical: 'basic.4y', 'basic.6y', 'basic.9y', 'high school', 'illiterate', 'professional course', 'university degree', 'unknown')</t>
+  </si>
+  <si>
+    <t>Has credit in default (yes, no, unknown)</t>
+  </si>
+  <si>
+    <t>Has housing loan (yes, no, unknown)</t>
+  </si>
+  <si>
+    <t>Has personal loan (yes, no, unknown)</t>
+  </si>
+  <si>
+    <t>Last contact day of week (mon, tue, wed, thu, fri)</t>
+  </si>
+  <si>
+    <t>Last contact month of year (mar, apr, may, jun, jul, aug, sep, oct, nov, dec)</t>
+  </si>
+  <si>
+    <t>Outcome of the previous marketing campaign (categorical: ‘failure’, ‘nonexistent’, ‘success’)</t>
+  </si>
+  <si>
+    <t>Target variable: Has the client subscribed a term deposit (yes, no)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +183,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -45,15 +219,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -66,6 +314,152 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rechteck 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FDE702B-335E-A1A2-6943-B2B58AAFED65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10163175" y="295275"/>
+          <a:ext cx="6248400" cy="1247775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Unknow = empty</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> = Nas</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-CH" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Nonexistent = maybe NA?</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> ( The interpretation of "nonexistent" as missing values (NA) depends on the specific analysis context. If the absence of a previous contact is considered important information and labeling it as "nonexistent" holds no real meaning, it may be reasonable to consider this state as NA. Otherwise, "nonexistent" can be regarded as a valid value reflecting the actual state of the dataset.)</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-CH" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +724,405 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4">
+        <v>40.020000000000003</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4">
+        <v>10.421250000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4">
+        <v>330</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4">
+        <v>80</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1731</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4">
+        <v>8597</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4">
+        <v>990</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4">
+        <v>990</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4">
+        <v>2.5680000000000001</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4">
+        <v>2.7700135000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4">
+        <v>0.49490109999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4">
+        <v>8.1890000000000004E-2</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4">
+        <v>1.5709597</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4">
+        <v>93.58</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4">
+        <v>0.57884000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4">
+        <v>-40.5</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4">
+        <v>4.6281979</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4">
+        <v>3.621</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4">
+        <v>1.7344474000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C7:H7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>